<commit_message>
ADD: stl file for stage body
</commit_message>
<xml_diff>
--- a/BOM/BOM.xlsx
+++ b/BOM/BOM.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\iromu\Documents\pico\RSP-02\BOM\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{288DFC13-3B6E-4399-A3B2-E3058AC2BD2A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ADB615F1-D7ED-40FB-804D-42BBCFE1263B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="53280" yWindow="420" windowWidth="21600" windowHeight="11310" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-103" yWindow="-103" windowWidth="27977" windowHeight="17812" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="28">
   <si>
     <t>No</t>
     <phoneticPr fontId="1"/>
@@ -115,10 +115,6 @@
     <phoneticPr fontId="1"/>
   </si>
   <si>
-    <t>Body</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
     <t>Coupling</t>
     <phoneticPr fontId="1"/>
   </si>
@@ -128,6 +124,18 @@
   </si>
   <si>
     <t>3D printer</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>Body_base</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>Body_table</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t xml:space="preserve">3D printer </t>
     <phoneticPr fontId="1"/>
   </si>
 </sst>
@@ -462,10 +470,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E11"/>
+  <dimension ref="A1:E12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D16" sqref="D16"/>
+      <selection activeCell="D11" sqref="D11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18.45"/>
@@ -577,7 +585,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="7" spans="1:5" ht="24.9">
+    <row r="7" spans="1:5">
       <c r="A7">
         <v>6</v>
       </c>
@@ -599,7 +607,7 @@
         <v>7</v>
       </c>
       <c r="B8" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C8">
         <v>1</v>
@@ -621,7 +629,7 @@
         <v>9</v>
       </c>
       <c r="B10" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C10">
         <v>1</v>
@@ -635,13 +643,27 @@
         <v>10</v>
       </c>
       <c r="B11" t="s">
-        <v>22</v>
+        <v>25</v>
       </c>
       <c r="C11" t="s">
         <v>6</v>
       </c>
       <c r="D11" t="s">
-        <v>25</v>
+        <v>27</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5">
+      <c r="A12">
+        <v>11</v>
+      </c>
+      <c r="B12" t="s">
+        <v>26</v>
+      </c>
+      <c r="C12" t="s">
+        <v>6</v>
+      </c>
+      <c r="D12" t="s">
+        <v>24</v>
       </c>
     </row>
   </sheetData>

</xml_diff>